<commit_message>
add: new Cards list analysis (imported from Google Drive: https://docs.google.com/spreadsheets/d/1OQAYdWOY2dhdnjVGGqx_NlSOnSvBfDpd-nKg32b-MZ0)
</commit_message>
<xml_diff>
--- a/cards/Underground Ventures (new).xlsx
+++ b/cards/Underground Ventures (new).xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="80">
   <si>
     <t>#</t>
   </si>
@@ -53,193 +53,205 @@
     <t>monster</t>
   </si>
   <si>
+    <t>mort-vivant</t>
+  </si>
+  <si>
+    <t>Squelette</t>
+  </si>
+  <si>
+    <t>F&gt;=2</t>
+  </si>
+  <si>
+    <t>PV -2</t>
+  </si>
+  <si>
+    <t>PV -1</t>
+  </si>
+  <si>
+    <t>Bouclier (sauvegarde 1 PV lors d'un combat)</t>
+  </si>
+  <si>
     <t>Gobelin</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>2-&gt;3</t>
   </si>
   <si>
+    <t>Zombie</t>
+  </si>
+  <si>
+    <t>F&gt;=1 &amp; P&gt;=1</t>
+  </si>
+  <si>
     <t>Orc</t>
   </si>
   <si>
+    <t>F -1 &amp; P -1</t>
+  </si>
+  <si>
+    <t>F -1 | P -1</t>
+  </si>
+  <si>
+    <t>Pièces</t>
+  </si>
+  <si>
+    <t>2 PO</t>
+  </si>
+  <si>
     <t>3-&gt;4</t>
   </si>
   <si>
     <t>Ogre</t>
   </si>
   <si>
+    <t>Goule</t>
+  </si>
+  <si>
+    <t>F&gt;=3 &amp; PV&gt;=2</t>
+  </si>
+  <si>
+    <t>Épée argentée</t>
+  </si>
+  <si>
+    <t>argenté</t>
+  </si>
+  <si>
+    <t>1 PO</t>
+  </si>
+  <si>
     <t>Troll</t>
   </si>
   <si>
+    <t>Vampire</t>
+  </si>
+  <si>
+    <t>PV&gt;=3 &amp; P&gt;=3 &amp; arme argentée</t>
+  </si>
+  <si>
+    <t>PV = 0 &amp; P -2</t>
+  </si>
+  <si>
+    <t>PV -3</t>
+  </si>
+  <si>
+    <t>Collier en or donnant un bonus permanent de 1 P</t>
+  </si>
+  <si>
     <t>piège</t>
   </si>
   <si>
     <t>Chute de rocher</t>
   </si>
   <si>
+    <t>10 PO</t>
+  </si>
+  <si>
+    <t>Volée de flechettes</t>
+  </si>
+  <si>
+    <t>F&gt;=3</t>
+  </si>
+  <si>
     <t>Fosse</t>
   </si>
   <si>
+    <t>P -1</t>
+  </si>
+  <si>
+    <t>poison</t>
+  </si>
+  <si>
+    <t>Brume empoisonnée</t>
+  </si>
+  <si>
+    <t>P&gt;=2</t>
+  </si>
+  <si>
     <t>Fosse de pieux</t>
   </si>
   <si>
+    <t>PV -1 &amp; P -1</t>
+  </si>
+  <si>
+    <t>Coffre + aiguille empoisonnée</t>
+  </si>
+  <si>
     <t>Plafond qui s'effondre</t>
   </si>
   <si>
+    <t>au choix</t>
+  </si>
+  <si>
+    <t>nil</t>
+  </si>
+  <si>
+    <t>PV -2 &amp; P -2</t>
+  </si>
+  <si>
+    <t>5 PO</t>
+  </si>
+  <si>
+    <t>maudit</t>
+  </si>
+  <si>
+    <t>Statuette maudite</t>
+  </si>
+  <si>
+    <t>P&gt;=4</t>
+  </si>
+  <si>
+    <t>F -1 permanent</t>
+  </si>
+  <si>
     <t>trésor</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Potion de soins</t>
   </si>
   <si>
+    <t>reward si test échoué uniquement, impossible de s'en débarasser volontairement</t>
+  </si>
+  <si>
+    <t>Potion de pouvoir</t>
+  </si>
+  <si>
+    <t>usage unique, P+2</t>
+  </si>
+  <si>
     <t>usage unique, PV +3</t>
   </si>
   <si>
+    <t>Arme sacralisée</t>
+  </si>
+  <si>
+    <t>sacré</t>
+  </si>
+  <si>
+    <t>permanent, P+1 pour les tests contre les morts-vivants</t>
+  </si>
+  <si>
+    <t>Diamant</t>
+  </si>
+  <si>
+    <t>amélioration</t>
+  </si>
+  <si>
     <t>Potion de guérison</t>
   </si>
   <si>
+    <t>événement</t>
+  </si>
+  <si>
+    <t>aventurier</t>
+  </si>
+  <si>
     <t>usage unique, full PV</t>
   </si>
   <si>
-    <t>mort-vivant</t>
-  </si>
-  <si>
-    <t>Squelette</t>
-  </si>
-  <si>
-    <t>F&gt;=2</t>
-  </si>
-  <si>
-    <t>PV -2</t>
-  </si>
-  <si>
-    <t>PV -1</t>
-  </si>
-  <si>
-    <t>Bouclier (sauvegarde 1 PV lors d'un combat)</t>
-  </si>
-  <si>
-    <t>Zombie</t>
-  </si>
-  <si>
-    <t>F&gt;=1 &amp; P&gt;=1</t>
-  </si>
-  <si>
-    <t>F -1 &amp; P -1</t>
-  </si>
-  <si>
-    <t>F -1 | P -1</t>
-  </si>
-  <si>
-    <t>Pièces</t>
-  </si>
-  <si>
-    <t>2 PO</t>
-  </si>
-  <si>
-    <t>Goule</t>
-  </si>
-  <si>
-    <t>F&gt;=3 &amp; PV&gt;=2</t>
-  </si>
-  <si>
-    <t>Épée argentée</t>
-  </si>
-  <si>
-    <t>argenté</t>
-  </si>
-  <si>
-    <t>1 PO</t>
-  </si>
-  <si>
-    <t>Vampire</t>
-  </si>
-  <si>
-    <t>PV&gt;=3 &amp; P&gt;=3 &amp; arme argentée</t>
-  </si>
-  <si>
-    <t>PV = 0 &amp; P -2</t>
-  </si>
-  <si>
-    <t>PV -3</t>
-  </si>
-  <si>
-    <t>Collier en or donnant un bonus permanent de 1 P</t>
-  </si>
-  <si>
-    <t>10 PO</t>
-  </si>
-  <si>
-    <t>Volée de flechettes</t>
-  </si>
-  <si>
-    <t>F&gt;=3</t>
-  </si>
-  <si>
-    <t>P -1</t>
-  </si>
-  <si>
-    <t>poison</t>
-  </si>
-  <si>
-    <t>Brume empoisonnée</t>
-  </si>
-  <si>
-    <t>P&gt;=2</t>
-  </si>
-  <si>
-    <t>PV -1 &amp; P -1</t>
-  </si>
-  <si>
-    <t>Coffre + aiguille empoisonnée</t>
-  </si>
-  <si>
-    <t>au choix</t>
-  </si>
-  <si>
-    <t>nil</t>
-  </si>
-  <si>
-    <t>PV -2 &amp; P -2</t>
-  </si>
-  <si>
-    <t>5 PO</t>
-  </si>
-  <si>
-    <t>maudit</t>
-  </si>
-  <si>
-    <t>Statuette maudite</t>
-  </si>
-  <si>
-    <t>P&gt;=4</t>
-  </si>
-  <si>
-    <t>F -1 permanent</t>
-  </si>
-  <si>
-    <t>reward si test échoué uniquement, impossible de s'en débarasser volontairement</t>
-  </si>
-  <si>
-    <t>Potion de pouvoir</t>
-  </si>
-  <si>
-    <t>usage unique, P+2</t>
-  </si>
-  <si>
-    <t>Arme sacralisée</t>
-  </si>
-  <si>
-    <t>sacré</t>
-  </si>
-  <si>
-    <t>permanent, P+1 pour les tests contre les morts-vivants</t>
-  </si>
-  <si>
-    <t>Diamant</t>
+    <t>escalier</t>
   </si>
 </sst>
 </file>
@@ -308,7 +320,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="2.14"/>
     <col customWidth="1" min="2" max="2" width="6.14"/>
-    <col customWidth="1" min="3" max="3" width="8.29"/>
+    <col customWidth="1" min="3" max="3" width="12.0"/>
     <col customWidth="1" min="4" max="4" width="10.86"/>
     <col customWidth="1" min="5" max="5" width="27.57"/>
     <col customWidth="1" min="6" max="6" width="29.86"/>
@@ -369,25 +381,25 @@
         <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L2" s="2"/>
     </row>
@@ -396,32 +408,32 @@
         <v>4.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="L3" s="2"/>
     </row>
@@ -430,34 +442,34 @@
         <v>2.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="L4" s="2"/>
     </row>
@@ -472,25 +484,25 @@
         <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L5" s="2"/>
     </row>
@@ -502,23 +514,23 @@
         <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -529,28 +541,28 @@
         <v>2.0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -561,32 +573,32 @@
         <v>1.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="L8" s="2"/>
     </row>
@@ -598,31 +610,31 @@
         <v>4.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="10">
@@ -633,30 +645,30 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11">
@@ -664,35 +676,35 @@
         <v>3.0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="12">
@@ -700,32 +712,32 @@
         <v>1.0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="L12" s="2"/>
     </row>
@@ -737,29 +749,101 @@
         <v>4.0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L13" s="2"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -783,9 +867,9 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="2.14"/>
     <col customWidth="1" min="2" max="2" width="6.14"/>
-    <col customWidth="1" min="3" max="3" width="8.29"/>
+    <col customWidth="1" min="3" max="3" width="12.0"/>
     <col customWidth="1" min="4" max="4" width="9.43"/>
-    <col customWidth="1" min="5" max="5" width="20.29"/>
+    <col customWidth="1" min="5" max="5" width="20.71"/>
     <col customWidth="1" min="6" max="6" width="9.0"/>
     <col customWidth="1" min="7" max="7" width="6.43"/>
     <col customWidth="1" min="8" max="8" width="8.29"/>
@@ -845,7 +929,7 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -860,14 +944,14 @@
         <v>4.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -882,14 +966,14 @@
         <v>2.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -911,7 +995,7 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -929,11 +1013,11 @@
         <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="1" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -948,14 +1032,14 @@
         <v>2.0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="1" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -970,14 +1054,14 @@
         <v>1.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="1" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -995,11 +1079,11 @@
         <v>4.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="1" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1017,27 +1101,27 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="1" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11">
@@ -1045,23 +1129,23 @@
         <v>3.0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1073,29 +1157,29 @@
         <v>1.0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13">
@@ -1106,25 +1190,97 @@
         <v>4.0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>